<commit_message>
Atualizacao ProductBacklog, criacao do fluxo do produto, adicionado Documento de Arquitetura e Licoes Aprendidas.
</commit_message>
<xml_diff>
--- a/documentos/ProductBacklog - Projeto.xlsx
+++ b/documentos/ProductBacklog - Projeto.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -65,23 +65,35 @@
     <t>Este requisito permite ao usuário com perfil de Visitante Visualizar Piso de um bloco.O sistema deve permitir que o usuário-cliente cadastre  remessas para cotações, devendo conter as seguintes informações: Tipo de mercadoria*, Peso Bruto, Quantidade de volumes ou de pallets, Valor Total da Mercadoria, Dimensões dos volumes, Endereço, Cidade Origem*, Prazo mínimo para pagamento de boleto, Nome da pessoa para contato, Telefone de contato, Dia da disponibilidade de coleta, Tempo de duração para receber lances*. O usuário-cliente deve optar por ser Emitente ou Destinatário. Caso o usuário-cliente não queira preencher todos os campos, poderá estar disponibilizando as informações através de anexo ou colar no campo Informações em formato texto. Todas as informações com * deverá ser preenchida obrigatoriamente.</t>
   </si>
   <si>
-    <t>UC.004 Manter Lance</t>
-  </si>
-  <si>
-    <t>O sistema deve permitir que o usuário-transportador manter lance em remessas postadas por usuário-cliente.</t>
-  </si>
-  <si>
     <t>UC.005 Visualizar Lances</t>
   </si>
   <si>
     <t>O sistema deve permitir que o usuário-cliente visualize todas os lances recebidos em sua remessa.</t>
+  </si>
+  <si>
+    <t>UC.006  Método Pagamento</t>
+  </si>
+  <si>
+    <t>UC.007 Iniciar Contrato</t>
+  </si>
+  <si>
+    <t>Este requisito tem como objetivo permitir que o usuário cliente inicie um contrato de frete a partir de um lance recebido em sua remessa.</t>
+  </si>
+  <si>
+    <t>Este requisito tem como objetivo permitir que o usuário cliente escolha uma forma de pagamento após iniciar um contrato de frete, podendo ser do tipo boleto, cartão de crédito ou débito.</t>
+  </si>
+  <si>
+    <t>UC.004 Emitir Lance</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que o usuário-transportador emite lance em remessas postadas por usuário-cliente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -110,6 +122,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Corbel"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -140,7 +162,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -174,6 +196,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -664,7 +707,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E7" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E9" totalsRowShown="0" dataDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="ITEM BP" dataDxfId="3"/>
     <tableColumn id="2" name="REQUISITOS" dataDxfId="2"/>
@@ -947,8 +990,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1022,10 +1065,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -1034,15 +1077,37 @@
         <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B9" s="18">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="16"/>
+    </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Atualizacao fluxo de processo e ProductBacklog.
</commit_message>
<xml_diff>
--- a/documentos/ProductBacklog - Projeto.xlsx
+++ b/documentos/ProductBacklog - Projeto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\OCF-Cargas\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.alves\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>ITEM BP</t>
-  </si>
-  <si>
-    <t>O sistema deve permitir que o usuário-cliente cadastre seus dados, sendo estes, CPF (não modificável), Nome Completo, Endereço, Número de endereço, Setor, Cidade, UF, CEP, Fone, Contato e E-mail de contato. Ao efetuar o cadastro, o usuário-cliente deve assinar o contrato via online e o sistema deve validar se o CPF é existente.</t>
   </si>
   <si>
     <t xml:space="preserve">UC.001 Manter Cliente
@@ -56,44 +53,41 @@
 </t>
   </si>
   <si>
-    <t>Este requisito permite ao usuário com perfil de Visitante Controlar O sistema deve permitir que o usuário-transportador cadastre e mantenha seus dados, sendo estes, CNPJ (não modificável), Razão Social, Nome Fantasia, Inscrição Estadual, Endereço, Número de endereço, Setor, Cidade, UF, CEP, Fone, Contato, E-mail de contato. Ao efetuar o cadastro, o usuário-transportador deve assinar o contrato via online e o sistema deve validar se o CNPJ é existente.o Mapa Geral do UniMAPS.</t>
-  </si>
-  <si>
     <t>UC.003 Manter Remessa</t>
   </si>
   <si>
-    <t>Este requisito permite ao usuário com perfil de Visitante Visualizar Piso de um bloco.O sistema deve permitir que o usuário-cliente cadastre  remessas para cotações, devendo conter as seguintes informações: Tipo de mercadoria*, Peso Bruto, Quantidade de volumes ou de pallets, Valor Total da Mercadoria, Dimensões dos volumes, Endereço, Cidade Origem*, Prazo mínimo para pagamento de boleto, Nome da pessoa para contato, Telefone de contato, Dia da disponibilidade de coleta, Tempo de duração para receber lances*. O usuário-cliente deve optar por ser Emitente ou Destinatário. Caso o usuário-cliente não queira preencher todos os campos, poderá estar disponibilizando as informações através de anexo ou colar no campo Informações em formato texto. Todas as informações com * deverá ser preenchida obrigatoriamente.</t>
-  </si>
-  <si>
     <t>UC.005 Visualizar Lances</t>
   </si>
   <si>
-    <t>O sistema deve permitir que o usuário-cliente visualize todas os lances recebidos em sua remessa.</t>
-  </si>
-  <si>
-    <t>UC.006  Método Pagamento</t>
-  </si>
-  <si>
     <t>UC.007 Iniciar Contrato</t>
   </si>
   <si>
-    <t>Este requisito tem como objetivo permitir que o usuário cliente inicie um contrato de frete a partir de um lance recebido em sua remessa.</t>
-  </si>
-  <si>
-    <t>Este requisito tem como objetivo permitir que o usuário cliente escolha uma forma de pagamento após iniciar um contrato de frete, podendo ser do tipo boleto, cartão de crédito ou débito.</t>
-  </si>
-  <si>
     <t>UC.004 Emitir Lance</t>
   </si>
   <si>
-    <t>O sistema deve permitir que o usuário-transportador emite lance em remessas postadas por usuário-cliente.</t>
+    <t>O sistema deve permitir que o usuário-transportador emite lance em remessas postadas por usuário-empresa.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que o usuário-empresa visualize todas os lances recebidos em sua remessa.</t>
+  </si>
+  <si>
+    <t>Este requisito tem como objetivo permitir que o usuário empresa inicie um contrato de frete a partir de um lance recebido em sua remessa.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que o usuário-empresa cadastre seus dados, sendo estes, CNPJ (não modificável), Razão Social, Endereço, Número de endereço, Setor, Cidade, UF, CEP, Fone, Contato e E-mail de contato. Ao efetuar o cadastro, o usuário-empresa deve assinar o contrato via online e o sistema deve validar se o CNPJ é existente.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que o usuário-transportador cadastre e mantenha seus dados, sendo estes, CNPJ (não modificável), Razão Social, Nome Fantasia, Inscrição Estadual, Endereço, Número de endereço, Setor, Cidade, UF, CEP, Fone, Contato, E-mail de contato. Ao efetuar o cadastro, o usuário-transportador deve assinar o contrato via online e o sistema deve validar se o CNPJ é existente.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir que o usuário-empresa cadastre  remessas para cotações, devendo conter as seguintes informações: Tipo de mercadoria*, Peso Bruto, Quantidade de volumes ou de pallets, Valor Total da Mercadoria, Dimensões dos volumes, Endereço, Cidade Origem*, Prazo mínimo para pagamento de boleto, Nome da pessoa para contato, Telefone de contato, Dia da disponibilidade de coleta, Tempo de duração para receber lances*. O usuário-empresa deve optar por ser Emitente ou Destinatário. Caso o usuário-empresa não queira preencher todos os campos, poderá estar disponibilizando as informações através de anexo ou colar no campo Informações em formato texto. Todas as informações com * deverá ser preenchida obrigatoriamente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -120,11 +114,6 @@
       <sz val="10"/>
       <name val="Corbel"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Corbel"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -162,7 +151,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -197,17 +186,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -707,7 +687,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E9" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E8" totalsRowShown="0" dataDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="ITEM BP" dataDxfId="3"/>
     <tableColumn id="2" name="REQUISITOS" dataDxfId="2"/>
@@ -988,10 +968,10 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1029,34 +1009,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -1065,10 +1045,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -1077,37 +1057,26 @@
         <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="15">
         <v>6</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="18">
-        <v>7</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="16"/>
-    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1089,6 @@
     <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Vision box, e atualizacao nos documentos
</commit_message>
<xml_diff>
--- a/documentos/ProductBacklog - Projeto.xlsx
+++ b/documentos/ProductBacklog - Projeto.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.alves\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="783"/>
   </bookViews>
@@ -20,8 +15,8 @@
     <definedName name="Área_Impressão_Agenda">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="Área_Impressão_Atribuição">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="IníciodoCronograma">#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product Backlog'!$2:$2</definedName>
     <definedName name="TérminoAgenda">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product Backlog'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -59,9 +54,6 @@
     <t>UC.005 Visualizar Lances</t>
   </si>
   <si>
-    <t>UC.007 Iniciar Contrato</t>
-  </si>
-  <si>
     <t>UC.004 Emitir Lance</t>
   </si>
   <si>
@@ -81,6 +73,9 @@
   </si>
   <si>
     <t>O sistema deve permitir que o usuário-empresa cadastre  remessas para cotações, devendo conter as seguintes informações: Tipo de mercadoria*, Peso Bruto, Quantidade de volumes ou de pallets, Valor Total da Mercadoria, Dimensões dos volumes, Endereço, Cidade Origem*, Prazo mínimo para pagamento de boleto, Nome da pessoa para contato, Telefone de contato, Dia da disponibilidade de coleta, Tempo de duração para receber lances*. O usuário-empresa deve optar por ser Emitente ou Destinatário. Caso o usuário-empresa não queira preencher todos os campos, poderá estar disponibilizando as informações através de anexo ou colar no campo Informações em formato texto. Todas as informações com * deverá ser preenchida obrigatoriamente.</t>
+  </si>
+  <si>
+    <t>UC.006 Iniciar Contrato</t>
   </si>
 </sst>
 </file>
@@ -151,14 +146,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -169,22 +161,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -193,17 +173,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
     <dxf>
       <font>
         <strike val="0"/>
@@ -216,6 +199,7 @@
         <name val="Corbel"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -242,7 +226,9 @@
         <name val="Corbel"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -602,28 +588,28 @@
   </dxfs>
   <tableStyles count="4" defaultTableStyle="Visão geral do semestre" defaultPivotStyle="Visão Geral do Semestre - Tabela Dinâmica">
     <tableStyle name="Estilo Dinâmico Leve 2 2" table="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="totalRow" dxfId="19"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="18"/>
     </tableStyle>
     <tableStyle name="Visão geral do semestre" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
     </tableStyle>
     <tableStyle name="Visão Geral do Semestre - Tabela Dinâmica" table="0" count="6">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="9"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstColumn" dxfId="12"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Visão Geral do Semestre - Tabela Dinâmica 2" table="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
-      <tableStyleElement type="headerRow" dxfId="6"/>
-      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="firstColumn" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -687,12 +673,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E8" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B2:E8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="5">
   <tableColumns count="4">
-    <tableColumn id="1" name="ITEM BP" dataDxfId="3"/>
-    <tableColumn id="2" name="REQUISITOS" dataDxfId="2"/>
+    <tableColumn id="1" name="ITEM BP" dataDxfId="2"/>
+    <tableColumn id="2" name="REQUISITOS" dataDxfId="0"/>
     <tableColumn id="3" name="DESCRIÇÃO" dataDxfId="1"/>
-    <tableColumn id="4" name="ESTIMATIVA (HORAS)" dataDxfId="0"/>
+    <tableColumn id="4" name="ESTIMATIVA (HORAS)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Visão geral do semestre" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -971,110 +957,110 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:5" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5"/>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="15">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>